<commit_message>
Final data analysis program in progress, subjects are automatically removed from the data pool if their control results were too large.
</commit_message>
<xml_diff>
--- a/example/results/subjectinfo.xlsx
+++ b/example/results/subjectinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterclark/Documents/GitHub/monophonic-flattening/example/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21929458-FA15-3B43-9B64-B12B918059DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87087BF3-FBC1-224F-AA23-2F8D8777930E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{BA651912-26D0-3540-A8E3-2921537D174B}"/>
   </bookViews>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3528ADF5-A009-C341-A1CB-0A4EF0D2E8A7}">
   <dimension ref="A1:AK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9:AJ9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,10 +601,7 @@
       <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="10">
-        <f ca="1">RAND()^6</f>
-        <v>2.6332808443873612E-4</v>
-      </c>
+      <c r="V4" s="10"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -631,54 +628,6 @@
       <c r="K5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="U5">
-        <v>1</v>
-      </c>
-      <c r="V5">
-        <v>2</v>
-      </c>
-      <c r="W5">
-        <v>3</v>
-      </c>
-      <c r="X5">
-        <v>4</v>
-      </c>
-      <c r="Y5">
-        <v>5</v>
-      </c>
-      <c r="Z5">
-        <v>6</v>
-      </c>
-      <c r="AA5">
-        <v>7</v>
-      </c>
-      <c r="AB5">
-        <v>8</v>
-      </c>
-      <c r="AC5">
-        <v>9</v>
-      </c>
-      <c r="AD5">
-        <v>10</v>
-      </c>
-      <c r="AE5">
-        <v>11</v>
-      </c>
-      <c r="AF5">
-        <v>12</v>
-      </c>
-      <c r="AG5">
-        <v>13</v>
-      </c>
-      <c r="AH5">
-        <v>14</v>
-      </c>
-      <c r="AI5">
-        <v>15</v>
-      </c>
-      <c r="AJ5">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -751,54 +700,22 @@
       <c r="G8" s="2">
         <v>3</v>
       </c>
-      <c r="U8" s="8">
-        <v>0.55118110200000003</v>
-      </c>
-      <c r="V8" s="8">
-        <v>0.51968503899999996</v>
-      </c>
-      <c r="W8" s="8">
-        <v>0.57480315000000004</v>
-      </c>
-      <c r="X8" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="8">
-        <v>0.716535433</v>
-      </c>
-      <c r="Z8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="8">
-        <v>0.582677165</v>
-      </c>
-      <c r="AB8" s="8">
-        <v>0.50393700799999996</v>
-      </c>
-      <c r="AC8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="8">
-        <v>0.65354330699999996</v>
-      </c>
-      <c r="AE8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="8">
-        <v>0.59842519699999996</v>
-      </c>
-      <c r="AJ8" s="8">
-        <v>0</v>
-      </c>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
       <c r="AK8" s="8"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
@@ -823,70 +740,22 @@
       <c r="G9" s="2">
         <v>4.5</v>
       </c>
-      <c r="U9" s="9">
-        <f ca="1">(U8+((-1)^U5)*V4)</f>
-        <v>0.55091777391556129</v>
-      </c>
-      <c r="V9" s="9">
-        <f t="shared" ref="V9:AJ9" si="0">(V8+((-1)^V5)*W4)</f>
-        <v>0.51968503899999996</v>
-      </c>
-      <c r="W9" s="9">
-        <f t="shared" si="0"/>
-        <v>0.57480315000000004</v>
-      </c>
-      <c r="X9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y9" s="9">
-        <f t="shared" si="0"/>
-        <v>0.716535433</v>
-      </c>
-      <c r="Z9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="9">
-        <f t="shared" si="0"/>
-        <v>0.582677165</v>
-      </c>
-      <c r="AB9" s="9">
-        <f t="shared" si="0"/>
-        <v>0.50393700799999996</v>
-      </c>
-      <c r="AC9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD9" s="9">
-        <f t="shared" si="0"/>
-        <v>0.65354330699999996</v>
-      </c>
-      <c r="AE9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AG9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AH9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI9" s="9">
-        <f t="shared" si="0"/>
-        <v>0.59842519699999996</v>
-      </c>
-      <c r="AJ9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -999,15 +868,15 @@
         <v>3.6666666666666665</v>
       </c>
       <c r="L13" s="7">
-        <f t="shared" ref="L13:N13" si="1">AVERAGE(E2:E22)</f>
+        <f t="shared" ref="L13:N13" si="0">AVERAGE(E2:E22)</f>
         <v>3.0952380952380953</v>
       </c>
       <c r="M13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="N13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.4523809523809526</v>
       </c>
     </row>
@@ -1041,15 +910,15 @@
         <v>1.3260216187277394</v>
       </c>
       <c r="L14" s="7">
-        <f t="shared" ref="L14:N14" si="2">STDEV(E2:E22)</f>
+        <f t="shared" ref="L14:N14" si="1">STDEV(E2:E22)</f>
         <v>1.7650711573407429</v>
       </c>
       <c r="M14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.0696215435033847</v>
       </c>
       <c r="N14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6874889770363086</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added true mean control error plot for alternate visualization.
</commit_message>
<xml_diff>
--- a/example/results/subjectinfo.xlsx
+++ b/example/results/subjectinfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterclark/Documents/GitHub/monophonic-flattening/example/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87087BF3-FBC1-224F-AA23-2F8D8777930E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020543EA-BDBD-1945-B48D-0CE5AC63E0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{BA651912-26D0-3540-A8E3-2921537D174B}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="Years">Sheet1!$K$2:$K$6</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>Participant</t>
   </si>
@@ -94,9 +93,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
-    <numFmt numFmtId="177" formatCode="0.0000000"/>
-    <numFmt numFmtId="179" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -127,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -137,16 +136,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +462,7 @@
   <dimension ref="A1:AK37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +523,7 @@
       <c r="D2" s="2">
         <v>1.5</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>0</v>
       </c>
       <c r="F2" s="2">
@@ -539,7 +537,7 @@
       </c>
       <c r="L2">
         <f>AVERAGE(B2:B40)</f>
-        <v>34.772727272727273</v>
+        <v>34.46153846153846</v>
       </c>
       <c r="M2">
         <f>COUNTIF(C2:C24,"M")</f>
@@ -571,9 +569,13 @@
       <c r="K3" s="3">
         <v>0.5</v>
       </c>
+      <c r="L3">
+        <f>STDEV(B2:B27)</f>
+        <v>12.722360690471779</v>
+      </c>
       <c r="M3">
         <f>COUNTIF(C3:C25,"F")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
@@ -601,7 +603,7 @@
       <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="10"/>
+      <c r="V4" s="8"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -700,23 +702,23 @@
       <c r="G8" s="2">
         <v>3</v>
       </c>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -740,22 +742,22 @@
       <c r="G9" s="2">
         <v>4.5</v>
       </c>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="9"/>
-      <c r="AF9" s="9"/>
-      <c r="AG9" s="9"/>
-      <c r="AH9" s="9"/>
-      <c r="AI9" s="9"/>
-      <c r="AJ9" s="9"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -863,21 +865,21 @@
       <c r="J13" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="7">
-        <f>AVERAGE(D2:D22)</f>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="L13" s="7">
-        <f t="shared" ref="L13:N13" si="0">AVERAGE(E2:E22)</f>
-        <v>3.0952380952380953</v>
-      </c>
-      <c r="M13" s="7">
-        <f t="shared" si="0"/>
-        <v>2.6666666666666665</v>
-      </c>
-      <c r="N13" s="7">
-        <f t="shared" si="0"/>
-        <v>2.4523809523809526</v>
+      <c r="K13" s="6">
+        <f>AVERAGE(D2:D27)</f>
+        <v>3.5576923076923075</v>
+      </c>
+      <c r="L13" s="6">
+        <f>AVERAGE(E2:E27)</f>
+        <v>2.9038461538461537</v>
+      </c>
+      <c r="M13" s="6">
+        <f>AVERAGE(F2:F27)</f>
+        <v>2.6730769230769229</v>
+      </c>
+      <c r="N13" s="6">
+        <f>AVERAGE(G2:G27)</f>
+        <v>2.4038461538461537</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.2">
@@ -905,21 +907,21 @@
       <c r="J14" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="7">
-        <f>STDEV(D2:D22)</f>
-        <v>1.3260216187277394</v>
-      </c>
-      <c r="L14" s="7">
-        <f t="shared" ref="L14:N14" si="1">STDEV(E2:E22)</f>
-        <v>1.7650711573407429</v>
-      </c>
-      <c r="M14" s="7">
-        <f t="shared" si="1"/>
-        <v>2.0696215435033847</v>
-      </c>
-      <c r="N14" s="7">
-        <f t="shared" si="1"/>
-        <v>1.6874889770363086</v>
+      <c r="K14" s="6">
+        <f>STDEV(D2:D27)</f>
+        <v>1.4375459858865254</v>
+      </c>
+      <c r="L14" s="6">
+        <f>STDEV(E2:E27)</f>
+        <v>1.8655788955132977</v>
+      </c>
+      <c r="M14" s="6">
+        <f>STDEV(F2:F27)</f>
+        <v>2.0973426410212883</v>
+      </c>
+      <c r="N14" s="6">
+        <f>STDEV(G2:G27)</f>
+        <v>1.6371880207797196</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.2">
@@ -1116,120 +1118,182 @@
       <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="D23" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E23" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="F23" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="G23" s="2">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="B24" s="1">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="F24" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="B25" s="1">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>35</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="F26" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>

</xml_diff>